<commit_message>
Db BackUp On 30-08-2021
Db BackUp On 30-08-2021
</commit_message>
<xml_diff>
--- a/DatabaseDocs/Docs/IncomeTax/ITAX.xlsx
+++ b/DatabaseDocs/Docs/IncomeTax/ITAX.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Monthly</t>
   </si>
@@ -390,7 +390,7 @@
   <dimension ref="B1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,7 +401,8 @@
     <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
@@ -445,21 +446,16 @@
         <f>C2-(D2+E2+F2)</f>
         <v>961600</v>
       </c>
-      <c r="H2" s="1">
-        <v>250000</v>
-      </c>
-      <c r="I2" s="2">
-        <f>G2-H2</f>
-        <v>711600</v>
-      </c>
-      <c r="J2" s="1">
-        <f>(20*I2)/100</f>
-        <v>142320</v>
-      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G4">
-        <v>109013</v>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2">
+        <v>961600</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>